<commit_message>
Added H7 board hardware and firmware
</commit_message>
<xml_diff>
--- a/Hardware/board_100pin/Orders/F7_100pin_BOM_JLC.xlsx
+++ b/Hardware/board_100pin/Orders/F7_100pin_BOM_JLC.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="89" documentId="8_{3463CFE6-4F20-4279-B039-57C24179BBDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BAD1DA50-FEEA-4FF2-8500-E99033D874B6}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="4180" windowWidth="28800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="2055" windowWidth="23040" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -1290,18 +1290,18 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>90</v>
       </c>

</xml_diff>